<commit_message>
Added load from json
</commit_message>
<xml_diff>
--- a/ER/ER Diagram.xlsx
+++ b/ER/ER Diagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiran/Documents/Flutter Apps/institute_objectbox/ER/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiran\Documents\Flutter Apps\batch_student_objectBox\ER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA43987-C9F1-1A48-9632-B46FD2464D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A1B3B2-0315-4F80-BC1A-4C18DD68EADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{8E5DD762-B25D-1442-A08F-3404545D8857}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E5DD762-B25D-1442-A08F-3404545D8857}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Batch</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Student_Course</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -166,14 +169,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -192,7 +209,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -480,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -490,209 +507,212 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA88D9D-7D52-2740-9120-C8ACA42FD4F2}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="299" zoomScaleNormal="299" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>98343434</v>
       </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>98453534</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>3</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>98435345</v>
       </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D6" s="1">
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>98776546</v>
       </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="G9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>2</v>
       </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D13" s="1">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D13" s="2">
         <v>3</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D14" s="1">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D14" s="2">
         <v>4</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>